<commit_message>
[JobClosing] : Initial Change
</commit_message>
<xml_diff>
--- a/TestData/JobcloseData.xlsx
+++ b/TestData/JobcloseData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
   <si>
     <t>Service</t>
   </si>
@@ -260,20 +260,35 @@
     <t>Job1</t>
   </si>
   <si>
-    <t>26-Jun-2023</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFE/00179/23-24</t>
-  </si>
-  <si>
-    <t>MUM/BKG/AEC/00012/2122-51</t>
+    <t>28-Jun-2023</t>
+  </si>
+  <si>
+    <t>Job2</t>
+  </si>
+  <si>
+    <t>Job3</t>
+  </si>
+  <si>
+    <t>Job4</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFE/00186/23-24</t>
+  </si>
+  <si>
+    <t>MUM/BKG/AEC/00012/2122-57</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFI/00187/23-24</t>
+  </si>
+  <si>
+    <t>MUM/BKG/AFIC/00014/2122-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +370,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -370,7 +391,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -608,12 +629,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -623,26 +668,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -653,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -693,9 +725,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -721,7 +750,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,10 +772,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -763,9 +791,17 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1049,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA9"/>
+  <dimension ref="A1:BA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,9 +1097,9 @@
     <col min="3" max="3" width="23.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
     <col min="11" max="11" width="16.5546875" customWidth="1"/>
@@ -1128,14 +1164,14 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="19" t="s">
         <v>0</v>
       </c>
       <c r="O3" s="11" t="s">
@@ -1214,90 +1250,90 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="O4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="P4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="17" t="s">
+      <c r="R4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="S4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="T4" s="17" t="s">
+      <c r="T4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="U4" s="17" t="s">
+      <c r="U4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="V4" s="17" t="s">
+      <c r="V4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="W4" s="17" t="s">
+      <c r="W4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="X4" s="17" t="s">
+      <c r="X4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="Y4" s="17" t="s">
+      <c r="Y4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="18" t="s">
+      <c r="Z4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="AA4" s="18" t="s">
+      <c r="AA4" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="AB4" s="18" t="s">
+      <c r="AB4" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AC4" s="18" t="s">
+      <c r="AC4" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AD4" s="18" t="s">
+      <c r="AD4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AE4" s="18" t="s">
+      <c r="AE4" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="AF4" s="18" t="s">
+      <c r="AF4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="AG4" s="18" t="s">
+      <c r="AG4" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AH4" s="18" t="s">
+      <c r="AH4" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AI4" s="19" t="s">
+      <c r="AI4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
-      <c r="AO4" s="16"/>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="16"/>
-      <c r="AR4" s="16"/>
-      <c r="AS4" s="16"/>
-      <c r="AT4" s="16"/>
-      <c r="AU4" s="16"/>
-      <c r="AV4" s="16"/>
-      <c r="AW4" s="16"/>
-      <c r="AX4" s="16"/>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="16"/>
-      <c r="BA4" s="16"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
+      <c r="AN4" s="15"/>
+      <c r="AO4" s="15"/>
+      <c r="AP4" s="15"/>
+      <c r="AQ4" s="15"/>
+      <c r="AR4" s="15"/>
+      <c r="AS4" s="15"/>
+      <c r="AT4" s="15"/>
+      <c r="AU4" s="15"/>
+      <c r="AV4" s="15"/>
+      <c r="AW4" s="15"/>
+      <c r="AX4" s="15"/>
+      <c r="AY4" s="15"/>
+      <c r="AZ4" s="15"/>
+      <c r="BA4" s="15"/>
     </row>
     <row r="5" spans="1:53" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
@@ -1314,67 +1350,67 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="R5" s="18" t="s">
+      <c r="R5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="S5" s="18" t="s">
+      <c r="S5" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="T5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="U5" s="18" t="s">
+      <c r="U5" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="V5" s="18" t="s">
+      <c r="V5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="W5" s="18" t="s">
+      <c r="W5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="X5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="Y5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="Z5" s="18" t="s">
+      <c r="Z5" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AA5" s="18" t="s">
+      <c r="AA5" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="AB5" s="18" t="s">
+      <c r="AB5" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="AC5" s="18" t="s">
+      <c r="AC5" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AD5" s="18" t="s">
+      <c r="AD5" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="AE5" s="18" t="s">
+      <c r="AE5" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="AF5" s="18" t="s">
+      <c r="AF5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="AG5" s="18" t="s">
+      <c r="AG5" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="AH5" s="19" t="s">
+      <c r="AH5" s="18" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1392,112 +1428,170 @@
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="32" t="s">
+      <c r="K7" s="30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:53" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:53" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="33">
         <v>1</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="34" t="s">
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:53" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:53" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="34">
         <v>2</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="27" t="s">
+      <c r="F9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" s="40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="B10" s="34">
+        <v>3</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="B11" s="34">
+        <v>4</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="K9" s="25"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="K11" s="40" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C11">
       <formula1>$O$3:$AH$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E11">
       <formula1>"Select,Mumbai,Chennai,DELHI,Bangalore"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F11">
       <formula1>$O$4:$AI$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G11">
       <formula1>$O$5:$AH$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[Job_Closing_Journal] : Alert popups handle
</commit_message>
<xml_diff>
--- a/TestData/JobcloseData.xlsx
+++ b/TestData/JobcloseData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="87">
   <si>
     <t>Service</t>
   </si>
@@ -272,9 +272,6 @@
     <t>Job4</t>
   </si>
   <si>
-    <t>CHN/BKG/AFE/00186/23-24</t>
-  </si>
-  <si>
     <t>MUM/BKG/AEC/00012/2122-57</t>
   </si>
   <si>
@@ -282,6 +279,12 @@
   </si>
   <si>
     <t>MUM/BKG/AFIC/00014/2122-16</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFE/00195/23-24</t>
+  </si>
+  <si>
+    <t>12-Jul-2023</t>
   </si>
 </sst>
 </file>
@@ -781,15 +784,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -802,6 +796,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1088,7 +1091,7 @@
   <dimension ref="A1:BA11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,11 +1167,11 @@
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="N3" s="19" t="s">
@@ -1470,9 +1473,9 @@
         <v>18</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="25" t="s">
@@ -1483,8 +1486,8 @@
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
-      <c r="J8" s="42" t="s">
-        <v>82</v>
+      <c r="J8" s="39" t="s">
+        <v>85</v>
       </c>
       <c r="K8" s="32" t="s">
         <v>77</v>
@@ -1503,7 +1506,7 @@
       <c r="D9" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F9" s="25" t="s">
@@ -1513,11 +1516,11 @@
         <v>59</v>
       </c>
       <c r="H9" s="23"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K9" s="40" t="s">
+      <c r="I9" s="36"/>
+      <c r="J9" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="37" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1531,7 +1534,7 @@
       <c r="D10" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F10" s="25" t="s">
@@ -1541,11 +1544,11 @@
         <v>60</v>
       </c>
       <c r="H10" s="23"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="40" t="s">
+      <c r="I10" s="36"/>
+      <c r="J10" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="37" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1559,7 +1562,7 @@
       <c r="D11" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="25" t="s">
@@ -1569,11 +1572,11 @@
         <v>58</v>
       </c>
       <c r="H11" s="23"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="K11" s="40" t="s">
+      <c r="I11" s="36"/>
+      <c r="J11" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="37" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>